<commit_message>
Added data type 'births_deaths' and uploaded to db.
</commit_message>
<xml_diff>
--- a/mySQL_Create/datagroups.xlsx
+++ b/mySQL_Create/datagroups.xlsx
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>